<commit_message>
IN-1017 visits API tests
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="980" windowWidth="31160" windowHeight="18420" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="720" yWindow="980" windowWidth="31160" windowHeight="18420" tabRatio="500" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="visit_outcome_reason_lookup" sheetId="8" r:id="rId8"/>
     <sheet name="visit_marked_lookup" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="148">
   <si>
     <t>mapping_file_name</t>
   </si>
@@ -305,9 +305,6 @@
     <t>Deputy Panel Assurance</t>
   </si>
   <si>
-    <t>Pro Team Section 58</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -452,9 +449,6 @@
     <t>VST-MED</t>
   </si>
   <si>
-    <t>VST-S58</t>
-  </si>
-  <si>
     <t>VST-CPRO</t>
   </si>
   <si>
@@ -486,7 +480,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -550,6 +544,18 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -589,8 +595,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -649,7 +659,11 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2278,7 +2292,7 @@
         <v>36</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K11" s="13"/>
       <c r="L11" s="10" t="s">
@@ -5493,8 +5507,8 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -5550,7 +5564,7 @@
         <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="19"/>
       <c r="F2" s="14"/>
@@ -5584,7 +5598,7 @@
         <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="14"/>
@@ -5618,7 +5632,7 @@
         <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="14"/>
@@ -5652,7 +5666,7 @@
         <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="14"/>
@@ -5686,7 +5700,7 @@
         <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="14"/>
@@ -5720,7 +5734,7 @@
         <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="14"/>
@@ -5785,7 +5799,7 @@
         <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="14"/>
@@ -5819,7 +5833,7 @@
         <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="14"/>
@@ -5853,7 +5867,7 @@
         <v>88</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="14"/>
@@ -5887,7 +5901,7 @@
         <v>89</v>
       </c>
       <c r="D12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="14"/>
@@ -5921,7 +5935,7 @@
         <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="14"/>
@@ -5955,7 +5969,7 @@
         <v>91</v>
       </c>
       <c r="D14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="14"/>
@@ -5985,11 +5999,11 @@
       <c r="B15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>92</v>
+      <c r="C15" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="14"/>
@@ -12183,16 +12197,16 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -12217,16 +12231,16 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
@@ -12251,16 +12265,16 @@
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="A4" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="14"/>
@@ -12285,16 +12299,16 @@
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="14"/>
@@ -18746,10 +18760,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -18780,10 +18794,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
@@ -18814,10 +18828,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="14"/>
@@ -25241,7 +25255,7 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -25290,10 +25304,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -25324,10 +25338,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
@@ -25358,10 +25372,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="14"/>
@@ -25392,10 +25406,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="14"/>
@@ -25426,10 +25440,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="14"/>
@@ -25460,10 +25474,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="14"/>
@@ -25494,10 +25508,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="14"/>
@@ -25528,10 +25542,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="14"/>
@@ -25562,10 +25576,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -25596,10 +25610,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -25630,10 +25644,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -25664,10 +25678,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -31916,7 +31930,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="14"/>
@@ -31947,7 +31961,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="14"/>
@@ -31978,7 +31992,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="14"/>
@@ -32009,7 +32023,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="14"/>
@@ -32040,10 +32054,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -32073,10 +32087,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
@@ -32106,10 +32120,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -32139,10 +32153,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -32172,10 +32186,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -32205,10 +32219,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -32238,10 +32252,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -32271,10 +32285,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -38308,14 +38322,14 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -38340,14 +38354,14 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
@@ -38372,7 +38386,7 @@
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>8</v>
@@ -38402,14 +38416,14 @@
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="14"/>

</xml_diff>

<commit_message>
IN-1017 visits API tests (#433)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="980" windowWidth="31160" windowHeight="18420" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="720" yWindow="980" windowWidth="31160" windowHeight="18420" tabRatio="500" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="visit_outcome_reason_lookup" sheetId="8" r:id="rId8"/>
     <sheet name="visit_marked_lookup" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="148">
   <si>
     <t>mapping_file_name</t>
   </si>
@@ -305,9 +305,6 @@
     <t>Deputy Panel Assurance</t>
   </si>
   <si>
-    <t>Pro Team Section 58</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -452,9 +449,6 @@
     <t>VST-MED</t>
   </si>
   <si>
-    <t>VST-S58</t>
-  </si>
-  <si>
     <t>VST-CPRO</t>
   </si>
   <si>
@@ -486,7 +480,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -550,6 +544,18 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -589,8 +595,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -649,7 +659,11 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2278,7 +2292,7 @@
         <v>36</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K11" s="13"/>
       <c r="L11" s="10" t="s">
@@ -5493,8 +5507,8 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -5550,7 +5564,7 @@
         <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="19"/>
       <c r="F2" s="14"/>
@@ -5584,7 +5598,7 @@
         <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="14"/>
@@ -5618,7 +5632,7 @@
         <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="14"/>
@@ -5652,7 +5666,7 @@
         <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="14"/>
@@ -5686,7 +5700,7 @@
         <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="14"/>
@@ -5720,7 +5734,7 @@
         <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="14"/>
@@ -5785,7 +5799,7 @@
         <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="14"/>
@@ -5819,7 +5833,7 @@
         <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="14"/>
@@ -5853,7 +5867,7 @@
         <v>88</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="14"/>
@@ -5887,7 +5901,7 @@
         <v>89</v>
       </c>
       <c r="D12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="14"/>
@@ -5921,7 +5935,7 @@
         <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="14"/>
@@ -5955,7 +5969,7 @@
         <v>91</v>
       </c>
       <c r="D14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="14"/>
@@ -5985,11 +5999,11 @@
       <c r="B15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>92</v>
+      <c r="C15" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="14"/>
@@ -12183,16 +12197,16 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -12217,16 +12231,16 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
@@ -12251,16 +12265,16 @@
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="A4" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="14"/>
@@ -12285,16 +12299,16 @@
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="14"/>
@@ -18746,10 +18760,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -18780,10 +18794,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
@@ -18814,10 +18828,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="14"/>
@@ -25241,7 +25255,7 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -25290,10 +25304,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -25324,10 +25338,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
@@ -25358,10 +25372,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="14"/>
@@ -25392,10 +25406,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="14"/>
@@ -25426,10 +25440,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="14"/>
@@ -25460,10 +25474,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="14"/>
@@ -25494,10 +25508,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="14"/>
@@ -25528,10 +25542,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="14"/>
@@ -25562,10 +25576,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -25596,10 +25610,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -25630,10 +25644,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -25664,10 +25678,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -31916,7 +31930,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="14"/>
@@ -31947,7 +31961,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="14"/>
@@ -31978,7 +31992,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="14"/>
@@ -32009,7 +32023,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="14"/>
@@ -32040,10 +32054,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -32073,10 +32087,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
@@ -32106,10 +32120,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -32139,10 +32153,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -32172,10 +32186,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -32205,10 +32219,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -32238,10 +32252,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -32271,10 +32285,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -38308,14 +38322,14 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -38340,14 +38354,14 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
@@ -38372,7 +38386,7 @@
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>8</v>
@@ -38402,14 +38416,14 @@
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="14"/>

</xml_diff>

<commit_message>
Wire up set_visits_visitsubtype table transform
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C253B634-3F50-6845-8F43-458122AC9244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B67EE8-82B2-3C43-9A6E-717594223821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="500" windowWidth="29980" windowHeight="18480" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="6480" windowWidth="29980" windowHeight="18480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="138">
   <si>
     <t>mapping_file_name</t>
   </si>
@@ -441,6 +441,12 @@
   <si>
     <t>Case, Report Type</t>
   </si>
+  <si>
+    <t>table_transforms</t>
+  </si>
+  <si>
+    <t>set_visits_visitsubtype = {"source_cols": ["Req By", "Report Type"], "target_cols": ["visitsubtype"]}</t>
+  </si>
 </sst>
 </file>
 
@@ -835,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -872,7 +878,9 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="1" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="12" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -892,6 +900,9 @@
       </c>
       <c r="H2" s="3" t="s">
         <v>135</v>
+      </c>
+      <c r="I2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12" customHeight="1"/>
@@ -18649,7 +18660,7 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
Fix lookup table for visit type
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B67EE8-82B2-3C43-9A6E-717594223821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5309231-6D0D-2940-8C4E-0AF7CB1BCB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="6480" windowWidth="29980" windowHeight="18480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="1920" windowWidth="29980" windowHeight="18480" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="1" r:id="rId1"/>
@@ -430,12 +430,6 @@
     <t>Categ</t>
   </si>
   <si>
-    <t xml:space="preserve"> VT-INV</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> VT-ASS</t>
-  </si>
-  <si>
     <t>Mapped in visits transform dependent on Req By and Report Type</t>
   </si>
   <si>
@@ -446,6 +440,12 @@
   </si>
   <si>
     <t>set_visits_visitsubtype = {"source_cols": ["Req By", "Report Type"], "target_cols": ["visitsubtype"]}</t>
+  </si>
+  <si>
+    <t>VT-ASS</t>
+  </si>
+  <si>
+    <t>VT-INV</t>
   </si>
 </sst>
 </file>
@@ -841,7 +841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -879,7 +879,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="12" customHeight="1">
@@ -899,10 +899,10 @@
         <v>10</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" t="s">
         <v>135</v>
-      </c>
-      <c r="I2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12" customHeight="1"/>
@@ -2464,7 +2464,7 @@
         <v>30</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="15.75" customHeight="1">
@@ -12015,8 +12015,8 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -12140,7 +12140,7 @@
         <v>78</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="14"/>
@@ -12310,7 +12310,7 @@
         <v>83</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="14"/>
@@ -12344,7 +12344,7 @@
         <v>84</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="14"/>
@@ -12378,7 +12378,7 @@
         <v>85</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="14"/>
@@ -12412,7 +12412,7 @@
         <v>86</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="14"/>
@@ -12446,7 +12446,7 @@
         <v>87</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="14"/>
@@ -12480,7 +12480,7 @@
         <v>88</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="14"/>
@@ -12514,7 +12514,7 @@
         <v>89</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="14"/>

</xml_diff>

<commit_message>
Update visit outcome lookup in mappings
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5309231-6D0D-2940-8C4E-0AF7CB1BCB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF61B029-18BE-5148-9781-AACD1DBA12A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1920" windowWidth="29980" windowHeight="18480" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="1920" windowWidth="29980" windowHeight="18480" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="139">
   <si>
     <t>mapping_file_name</t>
   </si>
@@ -447,6 +447,9 @@
   <si>
     <t>VT-INV</t>
   </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
 </sst>
 </file>
 
@@ -534,7 +537,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -557,11 +560,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -624,6 +642,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12015,7 +12035,7 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -18660,7 +18680,9 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -18703,18 +18725,16 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="14"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -18737,15 +18757,15 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>102</v>
+      <c r="C3" s="30" t="s">
+        <v>138</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="30" t="s">
         <v>103</v>
       </c>
       <c r="E3" s="20"/>
@@ -18776,11 +18796,11 @@
       <c r="B4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>104</v>
+      <c r="C4" s="30" t="s">
+        <v>105</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>101</v>
+      <c r="D4" s="30" t="s">
+        <v>106</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="14"/>
@@ -18805,18 +18825,18 @@
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>105</v>
+      <c r="C5" s="11" t="s">
+        <v>100</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>106</v>
+      <c r="D5" s="11" t="s">
+        <v>101</v>
       </c>
-      <c r="E5" s="20"/>
+      <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -18838,18 +18858,10 @@
       <c r="X5" s="14"/>
     </row>
     <row r="6" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A6" s="18">
-        <v>4</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>103</v>
-      </c>
+      <c r="A6" s="18"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="20"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -18872,18 +18884,10 @@
       <c r="X6" s="14"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A7" s="18">
-        <v>5</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>103</v>
-      </c>
+      <c r="A7" s="18"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="20"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -18906,19 +18910,11 @@
       <c r="X7" s="14"/>
     </row>
     <row r="8" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A8" s="18">
-        <v>6</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="E8" s="21"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="34"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -18940,19 +18936,11 @@
       <c r="X8" s="14"/>
     </row>
     <row r="9" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A9" s="18">
-        <v>7</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" s="22"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="35"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -18974,19 +18962,11 @@
       <c r="X9" s="14"/>
     </row>
     <row r="10" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A10" s="18">
-        <v>8</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="14"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -19008,18 +18988,10 @@
       <c r="X10" s="14"/>
     </row>
     <row r="11" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A11" s="18">
-        <v>9</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>101</v>
-      </c>
+      <c r="A11" s="18"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -19042,18 +19014,10 @@
       <c r="X11" s="14"/>
     </row>
     <row r="12" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A12" s="18">
-        <v>10</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>103</v>
-      </c>
+      <c r="A12" s="18"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -19076,18 +19040,10 @@
       <c r="X12" s="14"/>
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A13" s="18">
-        <v>11</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>103</v>
-      </c>
+      <c r="A13" s="18"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
@@ -25268,6 +25224,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X1000">
+    <sortCondition ref="A2:A1000"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>

<commit_message>
IN-1189 Update visit outcome lookup table (#615)
* Update visit outcome lookup in mappings

* Fix API tests for new visit outcome mapping
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5309231-6D0D-2940-8C4E-0AF7CB1BCB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF61B029-18BE-5148-9781-AACD1DBA12A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1920" windowWidth="29980" windowHeight="18480" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="1920" windowWidth="29980" windowHeight="18480" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="139">
   <si>
     <t>mapping_file_name</t>
   </si>
@@ -447,6 +447,9 @@
   <si>
     <t>VT-INV</t>
   </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
 </sst>
 </file>
 
@@ -534,7 +537,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -557,11 +560,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -624,6 +642,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12015,7 +12035,7 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -18660,7 +18680,9 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -18703,18 +18725,16 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="14"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -18737,15 +18757,15 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>102</v>
+      <c r="C3" s="30" t="s">
+        <v>138</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="30" t="s">
         <v>103</v>
       </c>
       <c r="E3" s="20"/>
@@ -18776,11 +18796,11 @@
       <c r="B4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>104</v>
+      <c r="C4" s="30" t="s">
+        <v>105</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>101</v>
+      <c r="D4" s="30" t="s">
+        <v>106</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="14"/>
@@ -18805,18 +18825,18 @@
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>105</v>
+      <c r="C5" s="11" t="s">
+        <v>100</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>106</v>
+      <c r="D5" s="11" t="s">
+        <v>101</v>
       </c>
-      <c r="E5" s="20"/>
+      <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -18838,18 +18858,10 @@
       <c r="X5" s="14"/>
     </row>
     <row r="6" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A6" s="18">
-        <v>4</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>103</v>
-      </c>
+      <c r="A6" s="18"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="20"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -18872,18 +18884,10 @@
       <c r="X6" s="14"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A7" s="18">
-        <v>5</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>103</v>
-      </c>
+      <c r="A7" s="18"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="20"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -18906,19 +18910,11 @@
       <c r="X7" s="14"/>
     </row>
     <row r="8" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A8" s="18">
-        <v>6</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="E8" s="21"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="34"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -18940,19 +18936,11 @@
       <c r="X8" s="14"/>
     </row>
     <row r="9" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A9" s="18">
-        <v>7</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" s="22"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="35"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -18974,19 +18962,11 @@
       <c r="X9" s="14"/>
     </row>
     <row r="10" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A10" s="18">
-        <v>8</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="14"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -19008,18 +18988,10 @@
       <c r="X10" s="14"/>
     </row>
     <row r="11" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A11" s="18">
-        <v>9</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>101</v>
-      </c>
+      <c r="A11" s="18"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -19042,18 +19014,10 @@
       <c r="X11" s="14"/>
     </row>
     <row r="12" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A12" s="18">
-        <v>10</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>103</v>
-      </c>
+      <c r="A12" s="18"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -19076,18 +19040,10 @@
       <c r="X12" s="14"/>
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A13" s="18">
-        <v>11</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>103</v>
-      </c>
+      <c r="A13" s="18"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
@@ -25268,6 +25224,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X1000">
+    <sortCondition ref="A2:A1000"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>

<commit_message>
IN-1181 fix KPI Visits MI report
visits.visiturgency - essential for the production of an exportable report in Sirius -  was not in the migration requirements.

We could not identify a suitable field to map from in casrec in the time available before migration and a decision was taken to set all visits to a default of ‘Standard’ (‘VU-STAN’)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF61B029-18BE-5148-9781-AACD1DBA12A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E2B676-19B5-0C49-BDAD-4AA5A4D1AB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1920" windowWidth="29980" windowHeight="18480" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="1920" windowWidth="40960" windowHeight="27160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="140">
   <si>
     <t>mapping_file_name</t>
   </si>
@@ -449,6 +449,9 @@
   </si>
   <si>
     <t>Cancelled</t>
+  </si>
+  <si>
+    <t>VU-STAN</t>
   </si>
 </sst>
 </file>
@@ -1933,9 +1936,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2507,8 +2510,11 @@
       <c r="J19" s="10"/>
       <c r="K19" s="13"/>
       <c r="L19" s="12"/>
+      <c r="M19" s="12" t="s">
+        <v>139</v>
+      </c>
       <c r="P19" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="Q19" s="8"/>
     </row>
@@ -18680,7 +18686,7 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
IN-1181 fix KPI Visits MI report (#617)
visits.visiturgency - essential for the production of an exportable report in Sirius -  was not in the migration requirements.

We could not identify a suitable field to map from in casrec in the time available before migration and a decision was taken to set all visits to a default of ‘Standard’ (‘VU-STAN’)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF61B029-18BE-5148-9781-AACD1DBA12A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E2B676-19B5-0C49-BDAD-4AA5A4D1AB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1920" windowWidth="29980" windowHeight="18480" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="1920" windowWidth="40960" windowHeight="27160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="140">
   <si>
     <t>mapping_file_name</t>
   </si>
@@ -449,6 +449,9 @@
   </si>
   <si>
     <t>Cancelled</t>
+  </si>
+  <si>
+    <t>VU-STAN</t>
   </si>
 </sst>
 </file>
@@ -1933,9 +1936,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2507,8 +2510,11 @@
       <c r="J19" s="10"/>
       <c r="K19" s="13"/>
       <c r="L19" s="12"/>
+      <c r="M19" s="12" t="s">
+        <v>139</v>
+      </c>
       <c r="P19" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="Q19" s="8"/>
     </row>
@@ -18680,7 +18686,7 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
IN-1192 Update visit mapping for reportduedate
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E2B676-19B5-0C49-BDAD-4AA5A4D1AB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8305E0-B884-D44B-B72C-5848855EF7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1920" windowWidth="40960" windowHeight="27160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>visitreportduedate</t>
-  </si>
-  <si>
-    <t>Commission Issued</t>
   </si>
   <si>
     <t>visitoutcome</t>
@@ -452,6 +449,9 @@
   </si>
   <si>
     <t>VU-STAN</t>
+  </si>
+  <si>
+    <t>Report Due</t>
   </si>
 </sst>
 </file>
@@ -902,7 +902,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="12" customHeight="1">
@@ -922,10 +922,10 @@
         <v>10</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12" customHeight="1"/>
@@ -1938,7 +1938,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2088,11 +2088,11 @@
         <v>35</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>30</v>
@@ -2169,8 +2169,8 @@
       <c r="H7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="10" t="s">
-        <v>42</v>
+      <c r="J7" s="30" t="s">
+        <v>139</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
@@ -2186,7 +2186,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>34</v>
@@ -2198,11 +2198,11 @@
         <v>35</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P8" s="8" t="s">
         <v>30</v>
@@ -2216,7 +2216,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>37</v>
@@ -2228,7 +2228,7 @@
         <v>35</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
@@ -2244,7 +2244,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>37</v>
@@ -2256,7 +2256,7 @@
         <v>35</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
@@ -2273,7 +2273,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>34</v>
@@ -2285,11 +2285,11 @@
         <v>35</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K11" s="13"/>
       <c r="L11" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>30</v>
@@ -2304,7 +2304,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>37</v>
@@ -2316,7 +2316,7 @@
         <v>35</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
@@ -2332,7 +2332,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>34</v>
@@ -2356,7 +2356,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>34</v>
@@ -2368,11 +2368,11 @@
         <v>35</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K14" s="13"/>
       <c r="L14" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P14" s="8" t="s">
         <v>30</v>
@@ -2387,7 +2387,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>37</v>
@@ -2399,7 +2399,7 @@
         <v>35</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
@@ -2415,7 +2415,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>37</v>
@@ -2427,7 +2427,7 @@
         <v>35</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
@@ -2443,7 +2443,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>37</v>
@@ -2455,7 +2455,7 @@
         <v>35</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
@@ -2471,7 +2471,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>34</v>
@@ -2487,7 +2487,7 @@
         <v>30</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="15.75" customHeight="1">
@@ -2498,7 +2498,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>34</v>
@@ -2511,7 +2511,7 @@
       <c r="K19" s="13"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P19" s="8" t="s">
         <v>30</v>
@@ -2526,7 +2526,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>34</v>
@@ -2538,11 +2538,11 @@
         <v>35</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K20" s="13"/>
       <c r="L20" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P20" s="8" t="s">
         <v>30</v>
@@ -4013,7 +4013,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>8</v>
@@ -4030,13 +4030,13 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>34</v>
@@ -5500,16 +5500,16 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
@@ -5534,16 +5534,16 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -5568,16 +5568,16 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
@@ -5602,16 +5602,16 @@
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="A4" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="14"/>
@@ -5636,16 +5636,16 @@
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="14"/>
@@ -12055,16 +12055,16 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
@@ -12095,10 +12095,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="19"/>
       <c r="F2" s="14"/>
@@ -12129,10 +12129,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="14"/>
@@ -12163,10 +12163,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="14"/>
@@ -12197,10 +12197,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="14"/>
@@ -12231,10 +12231,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="14"/>
@@ -12265,10 +12265,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="14"/>
@@ -12299,10 +12299,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="14"/>
@@ -12333,10 +12333,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="14"/>
@@ -12367,10 +12367,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="14"/>
@@ -12401,10 +12401,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="14"/>
@@ -12435,10 +12435,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="14"/>
@@ -12469,10 +12469,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="14"/>
@@ -12503,10 +12503,10 @@
         <v>8</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="14"/>
@@ -12537,10 +12537,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="14"/>
@@ -18697,16 +18697,16 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
@@ -18737,7 +18737,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="20"/>
@@ -18769,10 +18769,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
@@ -18803,10 +18803,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="14"/>
@@ -18837,10 +18837,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -25256,16 +25256,16 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
@@ -25295,7 +25295,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="14"/>
@@ -25326,7 +25326,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="14"/>
@@ -25357,7 +25357,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="14"/>
@@ -25388,7 +25388,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="14"/>
@@ -25419,10 +25419,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -25452,10 +25452,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
@@ -25485,10 +25485,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -25518,10 +25518,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -25551,10 +25551,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -25584,10 +25584,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -25617,10 +25617,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -25650,10 +25650,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -31650,16 +31650,16 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1">
       <c r="A1" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
@@ -31684,14 +31684,14 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -31716,14 +31716,14 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
@@ -31748,7 +31748,7 @@
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>8</v>
@@ -31778,14 +31778,14 @@
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="14"/>

</xml_diff>

<commit_message>
IN-1192 Update visit mapping for reportduedate (#648)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Visits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E2B676-19B5-0C49-BDAD-4AA5A4D1AB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8305E0-B884-D44B-B72C-5848855EF7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1920" windowWidth="40960" windowHeight="27160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>visitreportduedate</t>
-  </si>
-  <si>
-    <t>Commission Issued</t>
   </si>
   <si>
     <t>visitoutcome</t>
@@ -452,6 +449,9 @@
   </si>
   <si>
     <t>VU-STAN</t>
+  </si>
+  <si>
+    <t>Report Due</t>
   </si>
 </sst>
 </file>
@@ -902,7 +902,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="12" customHeight="1">
@@ -922,10 +922,10 @@
         <v>10</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12" customHeight="1"/>
@@ -1938,7 +1938,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2088,11 +2088,11 @@
         <v>35</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>30</v>
@@ -2169,8 +2169,8 @@
       <c r="H7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="10" t="s">
-        <v>42</v>
+      <c r="J7" s="30" t="s">
+        <v>139</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
@@ -2186,7 +2186,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>34</v>
@@ -2198,11 +2198,11 @@
         <v>35</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P8" s="8" t="s">
         <v>30</v>
@@ -2216,7 +2216,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>37</v>
@@ -2228,7 +2228,7 @@
         <v>35</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
@@ -2244,7 +2244,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>37</v>
@@ -2256,7 +2256,7 @@
         <v>35</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
@@ -2273,7 +2273,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>34</v>
@@ -2285,11 +2285,11 @@
         <v>35</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K11" s="13"/>
       <c r="L11" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>30</v>
@@ -2304,7 +2304,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>37</v>
@@ -2316,7 +2316,7 @@
         <v>35</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
@@ -2332,7 +2332,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>34</v>
@@ -2356,7 +2356,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>34</v>
@@ -2368,11 +2368,11 @@
         <v>35</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K14" s="13"/>
       <c r="L14" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P14" s="8" t="s">
         <v>30</v>
@@ -2387,7 +2387,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>37</v>
@@ -2399,7 +2399,7 @@
         <v>35</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
@@ -2415,7 +2415,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>37</v>
@@ -2427,7 +2427,7 @@
         <v>35</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
@@ -2443,7 +2443,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>37</v>
@@ -2455,7 +2455,7 @@
         <v>35</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
@@ -2471,7 +2471,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>34</v>
@@ -2487,7 +2487,7 @@
         <v>30</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="15.75" customHeight="1">
@@ -2498,7 +2498,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>34</v>
@@ -2511,7 +2511,7 @@
       <c r="K19" s="13"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P19" s="8" t="s">
         <v>30</v>
@@ -2526,7 +2526,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>34</v>
@@ -2538,11 +2538,11 @@
         <v>35</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K20" s="13"/>
       <c r="L20" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P20" s="8" t="s">
         <v>30</v>
@@ -4013,7 +4013,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>8</v>
@@ -4030,13 +4030,13 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>34</v>
@@ -5500,16 +5500,16 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
@@ -5534,16 +5534,16 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -5568,16 +5568,16 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
@@ -5602,16 +5602,16 @@
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="A4" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="14"/>
@@ -5636,16 +5636,16 @@
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="14"/>
@@ -12055,16 +12055,16 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
@@ -12095,10 +12095,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="19"/>
       <c r="F2" s="14"/>
@@ -12129,10 +12129,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="14"/>
@@ -12163,10 +12163,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="14"/>
@@ -12197,10 +12197,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="14"/>
@@ -12231,10 +12231,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="14"/>
@@ -12265,10 +12265,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="14"/>
@@ -12299,10 +12299,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="14"/>
@@ -12333,10 +12333,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="14"/>
@@ -12367,10 +12367,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="14"/>
@@ -12401,10 +12401,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="14"/>
@@ -12435,10 +12435,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="14"/>
@@ -12469,10 +12469,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="14"/>
@@ -12503,10 +12503,10 @@
         <v>8</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="14"/>
@@ -12537,10 +12537,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="14"/>
@@ -18697,16 +18697,16 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
@@ -18737,7 +18737,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="20"/>
@@ -18769,10 +18769,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
@@ -18803,10 +18803,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="14"/>
@@ -18837,10 +18837,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -25256,16 +25256,16 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1">
       <c r="A1" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
@@ -25295,7 +25295,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="14"/>
@@ -25326,7 +25326,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="14"/>
@@ -25357,7 +25357,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="14"/>
@@ -25388,7 +25388,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="14"/>
@@ -25419,10 +25419,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -25452,10 +25452,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
@@ -25485,10 +25485,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -25518,10 +25518,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -25551,10 +25551,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -25584,10 +25584,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -25617,10 +25617,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -25650,10 +25650,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -31650,16 +31650,16 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1">
       <c r="A1" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
@@ -31684,14 +31684,14 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -31716,14 +31716,14 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
@@ -31748,7 +31748,7 @@
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>8</v>
@@ -31778,14 +31778,14 @@
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="14"/>

</xml_diff>